<commit_message>
Add UnitOfWork all project
</commit_message>
<xml_diff>
--- a/Documents/Acciones.xlsx
+++ b/Documents/Acciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wwwda\source\repos\ElectionSystem\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36163C64-D52B-4FC6-AE55-EE55E10DD954}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C883497-2A9D-447F-AD78-EA1D60A12E83}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="1755" windowWidth="20730" windowHeight="11160" xr2:uid="{DB587FF0-7D4B-4F71-BECA-E11B3294D8E9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DB587FF0-7D4B-4F71-BECA-E11B3294D8E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
   <si>
     <t>USUARIO</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Asignar a otros Administradores</t>
   </si>
   <si>
-    <t>Borrar Evento</t>
-  </si>
-  <si>
     <t>Administrador Evento</t>
   </si>
   <si>
@@ -75,12 +72,6 @@
     <t>Votar</t>
   </si>
   <si>
-    <t>Borrar Candidato</t>
-  </si>
-  <si>
-    <t>Borrar Participante</t>
-  </si>
-  <si>
     <t>Registrame en eventos por código</t>
   </si>
   <si>
@@ -90,9 +81,6 @@
     <t>Asignar Candidatos</t>
   </si>
   <si>
-    <t>Borrar Administradores</t>
-  </si>
-  <si>
     <t>Consultar eventos en los que soy candidato</t>
   </si>
   <si>
@@ -115,6 +103,33 @@
   </si>
   <si>
     <t>Consultar Candidatos del evento por id</t>
+  </si>
+  <si>
+    <t>Actuvar o Desactivar Administradores</t>
+  </si>
+  <si>
+    <t>Actuvar o Desactivar Evento</t>
+  </si>
+  <si>
+    <t>Actuvar o Desactivar Candidato</t>
+  </si>
+  <si>
+    <t>Actuvar o Desactivar Participante</t>
+  </si>
+  <si>
+    <t>Registro Masivo</t>
+  </si>
+  <si>
+    <t>Carga imagen del Evento</t>
+  </si>
+  <si>
+    <t>Subir Imágenes</t>
+  </si>
+  <si>
+    <t>Borrar Imágenes</t>
+  </si>
+  <si>
+    <t>Incrementar Cantidad de Eventos</t>
   </si>
 </sst>
 </file>
@@ -156,11 +171,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B65DC9-1C1E-4BC0-9AD0-B5CBF88A800E}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="B13:D13"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -493,7 +507,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -507,7 +521,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -524,7 +538,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
@@ -541,7 +555,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
@@ -558,35 +572,35 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -594,22 +608,28 @@
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
-        <v>15</v>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>14</v>
+        <v>26</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -617,53 +637,73 @@
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" t="s">
-        <v>19</v>
+      <c r="A11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" t="s">
-        <v>20</v>
+        <v>34</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D13" t="s">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>